<commit_message>
Database is now saved into memory and can be recreated anytime easily. TODO: Write code for options 1-4 as in the project spec.
</commit_message>
<xml_diff>
--- a/src/main/java/edu/wpi/derbydemo/Museum_Database.xlsx
+++ b/src/main/java/edu/wpi/derbydemo/Museum_Database.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\IdeaProjects\testDB\src\main\java\edu\wpi\derbydemo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9AF9B6-273F-4E99-ADEA-199388765A90}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -207,49 +217,63 @@
   </si>
   <si>
     <t>Definitely Not an Alien</t>
+  </si>
+  <si>
+    <t>Visitors</t>
+  </si>
+  <si>
+    <t>Musee du Louvre, 75001 Paris, France</t>
+  </si>
+  <si>
+    <t>MARS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="DDG_ProximaNova"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF494949"/>
       <name val="DDG_ProximaNova"/>
     </font>
     <font>
-      <sz val="9.0"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF1D1E20"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
@@ -259,7 +283,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -269,66 +293,57 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -518,24 +533,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.0"/>
-    <col customWidth="1" min="2" max="2" width="51.86"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
+    <col min="2" max="2" width="51.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -560,10 +580,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="2">
-        <v>9600000.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>9600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -574,10 +594,10 @@
         <v>19</v>
       </c>
       <c r="D3" s="2">
-        <v>40000.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -588,10 +608,10 @@
         <v>19</v>
       </c>
       <c r="D4" s="2">
-        <v>90000.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -602,10 +622,10 @@
         <v>30</v>
       </c>
       <c r="D5" s="2">
-        <v>75000.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
@@ -616,28 +636,134 @@
         <v>37</v>
       </c>
       <c r="D6" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C56B3B6-3DE3-47C0-8F78-9E74E0738FB3}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="8">
+        <v>9600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.0"/>
+    <col min="1" max="1" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -651,7 +777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -665,7 +791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -679,7 +805,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -693,7 +819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -707,7 +833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -721,7 +847,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -735,7 +861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -749,7 +875,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -763,7 +889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -777,7 +903,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -791,7 +917,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -805,7 +931,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
@@ -819,7 +945,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -833,7 +959,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -847,7 +973,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -861,7 +987,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -875,7 +1001,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
         <v>32</v>
       </c>
@@ -889,7 +1015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
         <v>32</v>
       </c>
@@ -903,7 +1029,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -917,7 +1043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
         <v>32</v>
       </c>
@@ -932,6 +1058,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>